<commit_message>
add time-squared to models
</commit_message>
<xml_diff>
--- a/data/population_models/models_output_hainich.xlsx
+++ b/data/population_models/models_output_hainich.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,17 +412,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -432,29 +432,29 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~time)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G2">
-        <v>1847.627607508532</v>
+        <v>1871.070059855871</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.5013042621535068</v>
+        <v>0.5560908241250312</v>
       </c>
       <c r="J2">
-        <v>-10003.832</v>
+        <v>-9949.927799999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -464,7 +464,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -474,29 +474,29 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F3">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G3">
-        <v>1849.528704081633</v>
+        <v>1872.718959287532</v>
       </c>
       <c r="H3">
-        <v>1.901096573100176</v>
+        <v>1.648899431660766</v>
       </c>
       <c r="I3">
-        <v>0.1937686535302816</v>
+        <v>0.2438325984281831</v>
       </c>
       <c r="J3">
-        <v>-9985.636</v>
+        <v>-9950.2976</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -506,7 +506,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -516,39 +516,39 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F4">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>1851.64570204953</v>
+        <v>1874.650171186441</v>
       </c>
       <c r="H4">
-        <v>4.018094540997708</v>
+        <v>3.580111330569707</v>
       </c>
       <c r="I4">
-        <v>0.06723311816305533</v>
+        <v>0.09283985024564943</v>
       </c>
       <c r="J4">
-        <v>-10003.905</v>
+        <v>-9944.330599999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -558,39 +558,39 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F5">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="G5">
-        <v>1852.274731754161</v>
+        <v>1875.689959855871</v>
       </c>
       <c r="H5">
-        <v>4.647124245628902</v>
+        <v>4.619900000000143</v>
       </c>
       <c r="I5">
-        <v>0.04908979164040113</v>
+        <v>0.0552010311660396</v>
       </c>
       <c r="J5">
-        <v>-10001.229</v>
+        <v>-9945.3079</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -600,39 +600,39 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur + wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F6">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G6">
-        <v>1852.410131754161</v>
+        <v>1877.635071186441</v>
       </c>
       <c r="H6">
-        <v>4.782524245628792</v>
+        <v>6.565011330569632</v>
       </c>
       <c r="I6">
-        <v>0.04587641284539187</v>
+        <v>0.02087236360454426</v>
       </c>
       <c r="J6">
-        <v>-10001.094</v>
+        <v>-9941.345799999999</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -642,39 +642,39 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G7">
-        <v>1852.917107508532</v>
+        <v>1879.451759855871</v>
       </c>
       <c r="H7">
-        <v>5.289499999999862</v>
+        <v>8.381700000000137</v>
       </c>
       <c r="I7">
-        <v>0.03560418639946168</v>
+        <v>0.008415553775794837</v>
       </c>
       <c r="J7">
-        <v>-9998.541999999999</v>
+        <v>-9941.5461</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -684,39 +684,39 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F8">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G8">
-        <v>1853.275107508532</v>
+        <v>1880.439691105464</v>
       </c>
       <c r="H8">
-        <v>5.647499999999809</v>
+        <v>9.369631249592658</v>
       </c>
       <c r="I8">
-        <v>0.02976887029182239</v>
+        <v>0.005135185713077375</v>
       </c>
       <c r="J8">
-        <v>-9998.183999999999</v>
+        <v>-9936.525900000001</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -726,39 +726,39 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F9">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G9">
-        <v>1853.300731754161</v>
+        <v>1880.898971186441</v>
       </c>
       <c r="H9">
-        <v>5.673124245628742</v>
+        <v>9.828911330569554</v>
       </c>
       <c r="I9">
-        <v>0.02938990075570425</v>
+        <v>0.004081546531237779</v>
       </c>
       <c r="J9">
-        <v>-10000.203</v>
+        <v>-9938.081899999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -768,39 +768,39 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~1)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F10">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G10">
-        <v>1853.894227078891</v>
+        <v>1881.130191105464</v>
       </c>
       <c r="H10">
-        <v>6.266619570358671</v>
+        <v>10.06013124959259</v>
       </c>
       <c r="I10">
-        <v>0.02184350102245046</v>
+        <v>0.00363593394372025</v>
       </c>
       <c r="J10">
-        <v>-9995.522000000001</v>
+        <v>-9935.8354</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -810,39 +810,39 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F11">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G11">
-        <v>1854.542007508532</v>
+        <v>1882.304971186441</v>
       </c>
       <c r="H11">
-        <v>6.914399999999887</v>
+        <v>11.2349113305695</v>
       </c>
       <c r="I11">
-        <v>0.01580005192523281</v>
+        <v>0.00202076462772926</v>
       </c>
       <c r="J11">
-        <v>-9996.9172</v>
+        <v>-9936.6759</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -852,29 +852,29 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F12">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G12">
-        <v>1856.351008241291</v>
+        <v>1882.373071186441</v>
       </c>
       <c r="H12">
-        <v>8.723400732758819</v>
+        <v>11.30301133056969</v>
       </c>
       <c r="I12">
-        <v>0.006394977138071833</v>
+        <v>0.001953115848508479</v>
       </c>
       <c r="J12">
-        <v>-9974.7575</v>
+        <v>-9936.6077</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -894,39 +894,39 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F13">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G13">
-        <v>1858.319094220145</v>
+        <v>1882.723971186441</v>
       </c>
       <c r="H13">
-        <v>10.69148671161201</v>
+        <v>11.6539113305696</v>
       </c>
       <c r="I13">
-        <v>0.00239042188342868</v>
+        <v>0.001638819176821221</v>
       </c>
       <c r="J13">
-        <v>-9974.816699999999</v>
+        <v>-9936.2569</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -936,39 +936,39 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~time)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F14">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="G14">
-        <v>1859.23459151671</v>
+        <v>1882.743091105464</v>
       </c>
       <c r="H14">
-        <v>11.60698400817705</v>
+        <v>11.67303124959267</v>
       </c>
       <c r="I14">
-        <v>0.001512435434905725</v>
+        <v>0.001623226781928585</v>
       </c>
       <c r="J14">
-        <v>-10012.75</v>
+        <v>-9934.2225</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -978,39 +978,39 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F15">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>1868.233094220144</v>
+        <v>1882.800771186441</v>
       </c>
       <c r="H15">
-        <v>20.605486711612</v>
+        <v>11.73071133056965</v>
       </c>
       <c r="I15">
-        <v>1.68142232392388E-05</v>
+        <v>0.001577081470534858</v>
       </c>
       <c r="J15">
-        <v>-9964.902599999999</v>
+        <v>-9936.1801</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1020,39 +1020,39 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F16">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>1872.372794220144</v>
+        <v>1883.914859855871</v>
       </c>
       <c r="H16">
-        <v>24.74518671161195</v>
+        <v>12.84480000000008</v>
       </c>
       <c r="I16">
-        <v>2.12203418446241E-06</v>
+        <v>0.0009035097602042146</v>
       </c>
       <c r="J16">
-        <v>-9960.763000000001</v>
+        <v>-9937.082899999999</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1062,29 +1062,29 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F17">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G17">
-        <v>1872.391304081633</v>
+        <v>1888.490617442845</v>
       </c>
       <c r="H17">
-        <v>24.76369657310033</v>
+        <v>17.42055758697393</v>
       </c>
       <c r="I17">
-        <v>2.102485505418346E-06</v>
+        <v>9.168952294607485E-05</v>
       </c>
       <c r="J17">
-        <v>-9962.773499999999</v>
+        <v>-9926.4614</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1104,23 +1104,23 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + sundur)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F18">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G18">
-        <v>1873.562594220145</v>
+        <v>1888.951891105464</v>
       </c>
       <c r="H18">
-        <v>25.93498671161205</v>
+        <v>17.88183124959278</v>
       </c>
       <c r="I18">
-        <v>1.170551668955606E-06</v>
+        <v>7.280402832734477E-05</v>
       </c>
       <c r="J18">
-        <v>-9959.573200000001</v>
+        <v>-9928.0136</v>
       </c>
     </row>
     <row r="19">
@@ -1131,12 +1131,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~temp + sundur</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1146,39 +1146,39 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~time)N(~1)</t>
+          <t>Phi(~1)p(~temp + sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F19">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>1873.581408241291</v>
+        <v>1892.264791105464</v>
       </c>
       <c r="H19">
-        <v>25.95380073275896</v>
+        <v>21.19473124959268</v>
       </c>
       <c r="I19">
-        <v>1.159591907147251E-06</v>
+        <v>1.389211326133769E-05</v>
       </c>
       <c r="J19">
-        <v>-9957.527099999999</v>
+        <v>-9924.700800000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1188,39 +1188,39 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~1)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F20">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G20">
-        <v>1882.360243949045</v>
+        <v>1901.777271186441</v>
       </c>
       <c r="H20">
-        <v>34.73263644051212</v>
+        <v>30.70721133056963</v>
       </c>
       <c r="I20">
-        <v>1.438815882007276E-08</v>
+        <v>1.194426722731198E-07</v>
       </c>
       <c r="J20">
-        <v>-9946.722599999999</v>
+        <v>-9917.203600000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>~temp</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1230,29 +1230,29 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F21">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G21">
-        <v>1882.578608241291</v>
+        <v>1904.401359855871</v>
       </c>
       <c r="H21">
-        <v>34.95100073275898</v>
+        <v>33.33130000000006</v>
       </c>
       <c r="I21">
-        <v>1.289994977590547E-08</v>
+        <v>3.216221098937011E-08</v>
       </c>
       <c r="J21">
-        <v>-9948.5299</v>
+        <v>-9916.5964</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1272,39 +1272,39 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F22">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G22">
-        <v>1883.473094220145</v>
+        <v>1904.927271186441</v>
       </c>
       <c r="H22">
-        <v>35.84548671161201</v>
+        <v>33.85721133056973</v>
       </c>
       <c r="I22">
-        <v>8.248079856518091E-09</v>
+        <v>2.472553527295437E-08</v>
       </c>
       <c r="J22">
-        <v>-9949.6626</v>
+        <v>-9914.053599999999</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1314,39 +1314,39 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F23">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G23">
-        <v>1884.348708241291</v>
+        <v>1906.621291105464</v>
       </c>
       <c r="H23">
-        <v>36.72110073275894</v>
+        <v>35.55123124959277</v>
       </c>
       <c r="I23">
-        <v>5.323725914153728E-09</v>
+        <v>1.059970920043761E-08</v>
       </c>
       <c r="J23">
-        <v>-9946.7598</v>
+        <v>-9910.344300000001</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>~temp + wind</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1356,39 +1356,39 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~time)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F24">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G24">
-        <v>1884.598494220144</v>
+        <v>1906.932691105464</v>
       </c>
       <c r="H24">
-        <v>36.97088671161191</v>
+        <v>35.8626312495926</v>
       </c>
       <c r="I24">
-        <v>4.698674410391507E-09</v>
+        <v>9.071399633413308E-09</v>
       </c>
       <c r="J24">
-        <v>-9948.537200000001</v>
+        <v>-9910.0329</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1398,39 +1398,39 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~time)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F25">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G25">
-        <v>1886.247807508532</v>
+        <v>1907.864291105464</v>
       </c>
       <c r="H25">
-        <v>38.62019999999984</v>
+        <v>36.79423124959271</v>
       </c>
       <c r="I25">
-        <v>2.059830678249869E-09</v>
+        <v>5.693507934195166E-09</v>
       </c>
       <c r="J25">
-        <v>-9965.2114</v>
+        <v>-9909.1013</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>~sundur</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1440,39 +1440,39 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F26">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="G26">
-        <v>1890.371708241291</v>
+        <v>1909.879571186441</v>
       </c>
       <c r="H26">
-        <v>42.74410073275885</v>
+        <v>38.80951133056965</v>
       </c>
       <c r="I26">
-        <v>2.620220595576289E-10</v>
+        <v>2.078583238569972E-09</v>
       </c>
       <c r="J26">
-        <v>-9940.736800000001</v>
+        <v>-9909.1013</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1482,39 +1482,39 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~time)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F27">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G27">
-        <v>1893.713808241291</v>
+        <v>1910.744217442845</v>
       </c>
       <c r="H27">
-        <v>46.08620073275893</v>
+        <v>39.67415758697393</v>
       </c>
       <c r="I27">
-        <v>4.927311989713431E-11</v>
+        <v>1.348999758400227E-09</v>
       </c>
       <c r="J27">
-        <v>-9937.394700000001</v>
+        <v>-9904.2078</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~1</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~sundur + wind</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1524,39 +1524,39 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur + wind)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F28">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G28">
-        <v>1907.270208241291</v>
+        <v>1910.815191105464</v>
       </c>
       <c r="H28">
-        <v>59.64260073275886</v>
+        <v>39.74513124959276</v>
       </c>
       <c r="I28">
-        <v>5.608867811245317E-14</v>
+        <v>1.301967480396852E-09</v>
       </c>
       <c r="J28">
-        <v>-9923.838299999999</v>
+        <v>-9906.1504</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>~time</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~sundur</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1566,39 +1566,39 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Phi(~time)p(~1)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F29">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G29">
-        <v>1910.782343949045</v>
+        <v>1911.956091105464</v>
       </c>
       <c r="H29">
-        <v>63.15473644051212</v>
+        <v>40.88603124959263</v>
       </c>
       <c r="I29">
-        <v>9.687787988735678E-15</v>
+        <v>7.359644719840325E-10</v>
       </c>
       <c r="J29">
-        <v>-9918.3006</v>
+        <v>-9905.0095</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>~temp + wind + sundur</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1608,39 +1608,39 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G30">
-        <v>1975.486117442845</v>
+        <v>1912.173171186441</v>
       </c>
       <c r="H30">
-        <v>127.8585099343125</v>
+        <v>41.10311133056962</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>6.602653537226032E-10</v>
       </c>
       <c r="J30">
-        <v>-9839.465899999999</v>
+        <v>-9906.8076</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>~temp + sundur</t>
+          <t>~temp</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1650,29 +1650,29 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G31">
-        <v>2000.713548032163</v>
+        <v>1912.942191105464</v>
       </c>
       <c r="H31">
-        <v>153.0859405236301</v>
+        <v>41.87213124959271</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>4.49498198358713E-10</v>
       </c>
       <c r="J31">
-        <v>-9812.226500000001</v>
+        <v>-9904.0234</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1692,29 +1692,29 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G32">
-        <v>2013.825648032162</v>
+        <v>1912.963491105464</v>
       </c>
       <c r="H32">
-        <v>166.19804052363</v>
+        <v>41.8934312495926</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>4.447364438961549E-10</v>
       </c>
       <c r="J32">
-        <v>-9799.1145</v>
+        <v>-9904.0021</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1734,23 +1734,23 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
+          <t>Phi(~Time + I(Time^2))p(~temp)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F33">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G33">
-        <v>2031.80968071066</v>
+        <v>1914.268417442845</v>
       </c>
       <c r="H33">
-        <v>184.1820732021274</v>
+        <v>43.198357586974</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>2.316016053209092E-10</v>
       </c>
       <c r="J33">
-        <v>-9779.120199999999</v>
+        <v>-9900.6836</v>
       </c>
     </row>
     <row r="34">
@@ -1761,12 +1761,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>~sundur + wind</t>
+          <t>~temp + wind + sundur</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1776,23 +1776,23 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~Time)N(~1)</t>
         </is>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <v>2090.195748032162</v>
+        <v>1915.190491105464</v>
       </c>
       <c r="H34">
-        <v>242.5681405236296</v>
+        <v>44.12043124959268</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>1.460547929969907E-10</v>
       </c>
       <c r="J34">
-        <v>-9722.7444</v>
+        <v>-9901.775</v>
       </c>
     </row>
     <row r="35">
@@ -1808,7 +1808,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time + I(Time^2)</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1818,34 +1818,34 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
+          <t>Phi(~1)p(~sundur)pent(~Time + I(Time^2))N(~1)</t>
         </is>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G35">
-        <v>2103.91518071066</v>
+        <v>1918.742617442845</v>
       </c>
       <c r="H35">
-        <v>256.2875732021275</v>
+        <v>47.67255758697411</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>2.472756657839714E-11</v>
       </c>
       <c r="J35">
-        <v>-9707.014800000001</v>
+        <v>-9896.2094</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>~wind</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1860,39 +1860,39 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
+          <t>Phi(~Time)p(~temp + wind)pent(~1)N(~1)</t>
         </is>
       </c>
       <c r="F36">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>2109.09818071066</v>
+        <v>1920.672417442845</v>
       </c>
       <c r="H36">
-        <v>261.4705732021275</v>
+        <v>49.60235758697399</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>9.421729562654962E-12</v>
       </c>
       <c r="J36">
-        <v>-9701.8318</v>
+        <v>-9894.2796</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~temp + wind</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>~1</t>
+          <t>~Time</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1902,22 +1902,2290 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
+          <t>Phi(~Time)p(~temp + wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>1921.525691105464</v>
+      </c>
+      <c r="H37">
+        <v>50.45563124959267</v>
+      </c>
+      <c r="I37">
+        <v>6.149568063673517E-12</v>
+      </c>
+      <c r="J37">
+        <v>-9895.439899999999</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>~temp</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~temp)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>1923.777148032163</v>
+      </c>
+      <c r="H38">
+        <v>52.70708817629156</v>
+      </c>
+      <c r="I38">
+        <v>1.995018617649594E-12</v>
+      </c>
+      <c r="J38">
+        <v>-9889.163</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>~temp</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~temp)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F39">
+        <v>7</v>
+      </c>
+      <c r="G39">
+        <v>1925.141717442845</v>
+      </c>
+      <c r="H39">
+        <v>54.07165758697397</v>
+      </c>
+      <c r="I39">
+        <v>1.008403792378325E-12</v>
+      </c>
+      <c r="J39">
+        <v>-9889.810299999999</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>~temp + sundur</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + sundur)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F40">
+        <v>7</v>
+      </c>
+      <c r="G40">
+        <v>1926.998317442845</v>
+      </c>
+      <c r="H40">
+        <v>55.92825758697404</v>
+      </c>
+      <c r="I40">
+        <v>3.98546411161262E-13</v>
+      </c>
+      <c r="J40">
+        <v>-9887.9537</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>1932.516291105464</v>
+      </c>
+      <c r="H41">
+        <v>61.44623124959276</v>
+      </c>
+      <c r="I41">
+        <v>2.525027697037594E-14</v>
+      </c>
+      <c r="J41">
+        <v>-9884.4493</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>1933.620671186441</v>
+      </c>
+      <c r="H42">
+        <v>62.55061133056961</v>
+      </c>
+      <c r="I42">
+        <v>1.453627259911066E-14</v>
+      </c>
+      <c r="J42">
+        <v>-9885.360199999999</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>~sundur + wind</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~sundur + wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+      <c r="G43">
+        <v>1935.139817442845</v>
+      </c>
+      <c r="H43">
+        <v>64.06975758697399</v>
+      </c>
+      <c r="I43">
+        <v>6.801029216484696E-15</v>
+      </c>
+      <c r="J43">
+        <v>-9879.8122</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>~sundur</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~sundur)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+      <c r="G44">
+        <v>1936.790648032163</v>
+      </c>
+      <c r="H44">
+        <v>65.72058817629159</v>
+      </c>
+      <c r="I44">
+        <v>2.979211479877698E-15</v>
+      </c>
+      <c r="J44">
+        <v>-9876.1495</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>~sundur + wind</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~sundur + wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+      <c r="G45">
+        <v>1937.071991105464</v>
+      </c>
+      <c r="H45">
+        <v>66.00193124959264</v>
+      </c>
+      <c r="I45">
+        <v>2.588263337599737E-15</v>
+      </c>
+      <c r="J45">
+        <v>-9879.8935</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>~sundur</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~sundur)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F46">
+        <v>7</v>
+      </c>
+      <c r="G46">
+        <v>1938.599917442845</v>
+      </c>
+      <c r="H46">
+        <v>67.529857586974</v>
+      </c>
+      <c r="I46">
+        <v>1.205656167516912E-15</v>
+      </c>
+      <c r="J46">
+        <v>-9876.3521</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F47">
+        <v>8</v>
+      </c>
+      <c r="G47">
+        <v>1944.491491105464</v>
+      </c>
+      <c r="H47">
+        <v>73.42143124959262</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>-9872.474099999999</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F48">
+        <v>6</v>
+      </c>
+      <c r="G48">
+        <v>1946.166848032163</v>
+      </c>
+      <c r="H48">
+        <v>75.09678817629151</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>-9866.773300000001</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F49">
+        <v>7</v>
+      </c>
+      <c r="G49">
+        <v>1946.727717442845</v>
+      </c>
+      <c r="H49">
+        <v>75.65765758697398</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>-9868.2243</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50">
+        <v>1947.564391105464</v>
+      </c>
+      <c r="H50">
+        <v>76.49433124959273</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>-9869.4012</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F51">
+        <v>7</v>
+      </c>
+      <c r="G51">
+        <v>1947.754817442845</v>
+      </c>
+      <c r="H51">
+        <v>76.684757586974</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>-9867.197200000001</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F52">
+        <v>8</v>
+      </c>
+      <c r="G52">
+        <v>1947.793691105464</v>
+      </c>
+      <c r="H52">
+        <v>76.7236312495927</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>-9869.171899999999</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~1)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F53">
+        <v>7</v>
+      </c>
+      <c r="G53">
+        <v>1947.898417442845</v>
+      </c>
+      <c r="H53">
+        <v>76.82835758697411</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>-9867.053599999999</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F54">
+        <v>7</v>
+      </c>
+      <c r="G54">
+        <v>1948.037517442845</v>
+      </c>
+      <c r="H54">
+        <v>76.96745758697398</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>-9866.914500000001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>1948.212291105464</v>
+      </c>
+      <c r="H55">
+        <v>77.14223124959267</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>-9868.7533</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>~temp + wind</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + wind)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F56">
+        <v>8</v>
+      </c>
+      <c r="G56">
+        <v>1948.528591105464</v>
+      </c>
+      <c r="H56">
+        <v>77.45853124959262</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>-9868.437</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F57">
+        <v>8</v>
+      </c>
+      <c r="G57">
+        <v>1948.624991105464</v>
+      </c>
+      <c r="H57">
+        <v>77.55493124959276</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>-9868.3406</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F58">
+        <v>9</v>
+      </c>
+      <c r="G58">
+        <v>1948.946471186441</v>
+      </c>
+      <c r="H58">
+        <v>77.87641133056968</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>-9870.0344</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F59">
+        <v>8</v>
+      </c>
+      <c r="G59">
+        <v>1949.747191105464</v>
+      </c>
+      <c r="H59">
+        <v>78.67713124959278</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>-9867.2184</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F60">
+        <v>9</v>
+      </c>
+      <c r="G60">
+        <v>1950.161971186441</v>
+      </c>
+      <c r="H60">
+        <v>79.0919113305697</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <v>-9868.8189</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F61">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>1950.321071186441</v>
+      </c>
+      <c r="H61">
+        <v>79.25101133056955</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>-9868.659799999999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~Time + I(Time^2))pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F62">
+        <v>10</v>
+      </c>
+      <c r="G62">
+        <v>1951.815359855871</v>
+      </c>
+      <c r="H62">
+        <v>80.74530000000004</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>-9869.182500000001</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F63">
+        <v>7</v>
+      </c>
+      <c r="G63">
+        <v>1951.820317442845</v>
+      </c>
+      <c r="H63">
+        <v>80.75025758697393</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <v>-9863.1317</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>~sundur + wind</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~sundur + wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F64">
+        <v>7</v>
+      </c>
+      <c r="G64">
+        <v>1951.957217442845</v>
+      </c>
+      <c r="H64">
+        <v>80.8871575869739</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>-9862.994699999999</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>~temp</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F65">
+        <v>7</v>
+      </c>
+      <c r="G65">
+        <v>1953.136917442845</v>
+      </c>
+      <c r="H65">
+        <v>82.06685758697404</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>-9861.8151</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~1)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F66">
+        <v>6</v>
+      </c>
+      <c r="G66">
+        <v>1953.379548032163</v>
+      </c>
+      <c r="H66">
+        <v>82.30948817629155</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>-9859.560600000001</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F67">
+        <v>7</v>
+      </c>
+      <c r="G67">
+        <v>1955.279117442845</v>
+      </c>
+      <c r="H67">
+        <v>84.20905758697404</v>
+      </c>
+      <c r="I67">
+        <v>0</v>
+      </c>
+      <c r="J67">
+        <v>-9859.6729</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>~sundur</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~sundur)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F68">
+        <v>6</v>
+      </c>
+      <c r="G68">
+        <v>1956.777348032163</v>
+      </c>
+      <c r="H68">
+        <v>85.70728817629151</v>
+      </c>
+      <c r="I68">
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <v>-9856.1628</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~1)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F69">
+        <v>6</v>
+      </c>
+      <c r="G69">
+        <v>1959.193448032162</v>
+      </c>
+      <c r="H69">
+        <v>88.12338817629143</v>
+      </c>
+      <c r="I69">
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <v>-9853.7467</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~Time)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F70">
+        <v>7</v>
+      </c>
+      <c r="G70">
+        <v>1960.128017442845</v>
+      </c>
+      <c r="H70">
+        <v>89.057957586974</v>
+      </c>
+      <c r="I70">
+        <v>0</v>
+      </c>
+      <c r="J70">
+        <v>-9854.824000000001</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Phi(~Time + I(Time^2))p(~wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F71">
+        <v>7</v>
+      </c>
+      <c r="G71">
+        <v>1960.370917442845</v>
+      </c>
+      <c r="H71">
+        <v>89.30085758697396</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>-9854.581099999999</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F72">
+        <v>6</v>
+      </c>
+      <c r="G72">
+        <v>1963.050148032162</v>
+      </c>
+      <c r="H72">
+        <v>91.98008817629147</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>-9849.889999999999</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~1)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F73">
+        <v>5</v>
+      </c>
+      <c r="G73">
+        <v>1963.24728071066</v>
+      </c>
+      <c r="H73">
+        <v>92.17722085478886</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>-9847.682699999999</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Phi(~Time)p(~Time)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F74">
+        <v>6</v>
+      </c>
+      <c r="G74">
+        <v>1964.300148032162</v>
+      </c>
+      <c r="H74">
+        <v>93.23008817629147</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>-9848.639999999999</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F75">
+        <v>7</v>
+      </c>
+      <c r="G75">
+        <v>1971.677017442845</v>
+      </c>
+      <c r="H75">
+        <v>100.606957586974</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>-9843.275</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>~temp + wind</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F76">
+        <v>7</v>
+      </c>
+      <c r="G76">
+        <v>1972.580817442845</v>
+      </c>
+      <c r="H76">
+        <v>101.510757586974</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>-9842.3712</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>~temp + wind + sundur</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + wind + sundur)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F77">
+        <v>7</v>
+      </c>
+      <c r="G77">
+        <v>1975.486117442845</v>
+      </c>
+      <c r="H77">
+        <v>104.4160575869739</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>-9839.465899999999</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~wind)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F78">
+        <v>7</v>
+      </c>
+      <c r="G78">
+        <v>1978.364217442845</v>
+      </c>
+      <c r="H78">
+        <v>107.2941575869741</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>-9836.587799999999</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>~Time + I(Time^2)</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~1)pent(~Time + I(Time^2))N(~1)</t>
+        </is>
+      </c>
+      <c r="F79">
+        <v>6</v>
+      </c>
+      <c r="G79">
+        <v>1979.357348032162</v>
+      </c>
+      <c r="H79">
+        <v>108.2872881762914</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>-9833.5828</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>~temp</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F80">
+        <v>6</v>
+      </c>
+      <c r="G80">
+        <v>1979.992548032163</v>
+      </c>
+      <c r="H80">
+        <v>108.9224881762916</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>-9832.9476</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F81">
+        <v>6</v>
+      </c>
+      <c r="G81">
+        <v>1999.428348032163</v>
+      </c>
+      <c r="H81">
+        <v>128.3582881762916</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>-9813.5118</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~wind)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F82">
+        <v>6</v>
+      </c>
+      <c r="G82">
+        <v>2000.448248032163</v>
+      </c>
+      <c r="H82">
+        <v>129.3781881762916</v>
+      </c>
+      <c r="I82">
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>-9812.491900000001</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>~temp + sundur</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + sundur)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F83">
+        <v>6</v>
+      </c>
+      <c r="G83">
+        <v>2000.713548032163</v>
+      </c>
+      <c r="H83">
+        <v>129.6434881762916</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>-9812.226500000001</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~1)pent(~Time)N(~1)</t>
+        </is>
+      </c>
+      <c r="F84">
+        <v>5</v>
+      </c>
+      <c r="G84">
+        <v>2003.91698071066</v>
+      </c>
+      <c r="H84">
+        <v>132.8469208547888</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>-9807.013000000001</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>~temp + wind</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp + wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F85">
+        <v>6</v>
+      </c>
+      <c r="G85">
+        <v>2013.825648032162</v>
+      </c>
+      <c r="H85">
+        <v>142.7555881762914</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>-9799.1145</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>~Time</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~Time)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86">
+        <v>2031.47658071066</v>
+      </c>
+      <c r="H86">
+        <v>160.4065208547888</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>-9779.4534</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>~temp</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~temp)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F87">
+        <v>5</v>
+      </c>
+      <c r="G87">
+        <v>2031.80968071066</v>
+      </c>
+      <c r="H87">
+        <v>160.7396208547889</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>-9779.120199999999</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>~sundur + wind</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~sundur + wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F88">
+        <v>6</v>
+      </c>
+      <c r="G88">
+        <v>2090.195748032162</v>
+      </c>
+      <c r="H88">
+        <v>219.1256881762911</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>-9722.7444</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>~sundur</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~sundur)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F89">
+        <v>5</v>
+      </c>
+      <c r="G89">
+        <v>2103.91518071066</v>
+      </c>
+      <c r="H89">
+        <v>232.845120854789</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <v>-9707.014800000001</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>~wind</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Phi(~1)p(~wind)pent(~1)N(~1)</t>
+        </is>
+      </c>
+      <c r="F90">
+        <v>5</v>
+      </c>
+      <c r="G90">
+        <v>2109.09818071066</v>
+      </c>
+      <c r="H90">
+        <v>238.028120854789</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>-9701.8318</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>~1</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
           <t>Phi(~1)p(~1)pent(~1)N(~1)</t>
         </is>
       </c>
-      <c r="F37">
+      <c r="F91">
         <v>4</v>
       </c>
-      <c r="G37">
+      <c r="G91">
         <v>2121.399013319239</v>
       </c>
-      <c r="H37">
-        <v>273.7714058107063</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
+      <c r="H91">
+        <v>250.3289534633677</v>
+      </c>
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
         <v>-9687.522499999999</v>
       </c>
     </row>

</xml_diff>